<commit_message>
Latest code with all modules
</commit_message>
<xml_diff>
--- a/ShareAppV2/src/com/share/testdata/TestDataSheet.xlsx
+++ b/ShareAppV2/src/com/share/testdata/TestDataSheet.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7569B2B0-AFDF-4AE5-9185-DB3858A6F9BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thi1907501\git\ShareAppV2\ShareAppV2\src\com\share\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1187DE-67C3-49CF-ABB3-897F074D4233}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="19068" windowHeight="13224" activeTab="1" xr2:uid="{AC1E8FC1-B97C-4DB0-B2CE-53C9679652AA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AC1E8FC1-B97C-4DB0-B2CE-53C9679652AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +22,6 @@
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:G11"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="212">
   <si>
     <t>UserName</t>
   </si>
@@ -218,9 +222,6 @@
     <t>Test@1234</t>
   </si>
   <si>
-    <t>rams.shana+82@gmail.com</t>
-  </si>
-  <si>
     <t>+91</t>
   </si>
   <si>
@@ -326,9 +327,6 @@
     <t>testgamil.com</t>
   </si>
   <si>
-    <t>sit21@yopmail.com</t>
-  </si>
-  <si>
     <t>45Smit@jj</t>
   </si>
   <si>
@@ -353,9 +351,6 @@
     <t>2016</t>
   </si>
   <si>
-    <t>smuserqa1@yopmail.com</t>
-  </si>
-  <si>
     <t>Test@123</t>
   </si>
   <si>
@@ -428,9 +423,6 @@
     <t>9078</t>
   </si>
   <si>
-    <t>Test@1</t>
-  </si>
-  <si>
     <t>Justi</t>
   </si>
   <si>
@@ -440,9 +432,6 @@
     <t>987895756</t>
   </si>
   <si>
-    <t>Test@one</t>
-  </si>
-  <si>
     <t>Alex</t>
   </si>
   <si>
@@ -536,9 +525,6 @@
     <t>2ae14a90803f7ece</t>
   </si>
   <si>
-    <t>smtestqa2@yopmail.com</t>
-  </si>
-  <si>
     <t>existingPin</t>
   </si>
   <si>
@@ -549,6 +535,138 @@
   </si>
   <si>
     <t>1233</t>
+  </si>
+  <si>
+    <t>sharetest372@yopmail.com</t>
+  </si>
+  <si>
+    <t>AnotherGroupMember</t>
+  </si>
+  <si>
+    <t>arthurrimbaud@yopmail.com</t>
+  </si>
+  <si>
+    <t>Family head</t>
+  </si>
+  <si>
+    <t>Head password</t>
+  </si>
+  <si>
+    <t>sharetest369@yopmail.com</t>
+  </si>
+  <si>
+    <t>sharetest371@yopmail.com</t>
+  </si>
+  <si>
+    <t>FamilyMember</t>
+  </si>
+  <si>
+    <t>MemberPassword</t>
+  </si>
+  <si>
+    <t>Test@8544</t>
+  </si>
+  <si>
+    <t>Lam</t>
+  </si>
+  <si>
+    <t>TT</t>
+  </si>
+  <si>
+    <t>Peterherz</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>5566556644</t>
+  </si>
+  <si>
+    <t>99950569412</t>
+  </si>
+  <si>
+    <t>999505694</t>
+  </si>
+  <si>
+    <t>cCode</t>
+  </si>
+  <si>
+    <t>+971</t>
+  </si>
+  <si>
+    <t>Test@12</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>Testingone</t>
+  </si>
+  <si>
+    <t>email clear</t>
+  </si>
+  <si>
+    <t>email re-enter</t>
+  </si>
+  <si>
+    <t>clearEmail</t>
+  </si>
+  <si>
+    <t>reEnterEmail</t>
+  </si>
+  <si>
+    <t>rams.shana+222@gmail.com</t>
+  </si>
+  <si>
+    <t>rams.shana+224@gmail.com</t>
+  </si>
+  <si>
+    <t>smtestqa13@yopmail.com</t>
+  </si>
+  <si>
+    <t>VisaCardNumber</t>
+  </si>
+  <si>
+    <t>VisaNameOnCard</t>
+  </si>
+  <si>
+    <t>VisaCardExpiry</t>
+  </si>
+  <si>
+    <t>VisaCardCVC</t>
+  </si>
+  <si>
+    <t>TransactionUser</t>
+  </si>
+  <si>
+    <t>TransactionUserPassword</t>
+  </si>
+  <si>
+    <t>4111 1111 1111 1111</t>
+  </si>
+  <si>
+    <t>Lorem Iya</t>
+  </si>
+  <si>
+    <t>automation10@yopmail.com</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>modifyEmail</t>
+  </si>
+  <si>
+    <t>rams.shana+93@gmail.com</t>
+  </si>
+  <si>
+    <t>smautomation08@yopmail.com</t>
+  </si>
+  <si>
+    <t>rams.shana+1002@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -634,7 +752,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -651,6 +769,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -969,15 +1091,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6644A30B-D8F6-4A82-9CDE-322859A69DF6}">
-  <dimension ref="A1:BI3"/>
+  <dimension ref="A1:BS6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AJ2" sqref="AJ2"/>
+    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
+      <selection activeCell="BI2" sqref="BI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="47" max="47" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="16" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="22.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:61">
+    <row r="1" spans="1:71">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1030,139 +1164,169 @@
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AY1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BB1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BD1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BL1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BM1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:61" ht="15" thickBot="1">
+      <c r="BN1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>199</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>200</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>201</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:71" ht="15" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>61</v>
       </c>
@@ -1170,34 +1334,34 @@
         <v>62</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>62</v>
@@ -1206,166 +1370,217 @@
         <v>62</v>
       </c>
       <c r="O2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="R2" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="T2" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="U2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="V2" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="W2" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="X2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="Y2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="AA2" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="AB2" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="Z2" s="8" t="s">
+      <c r="AC2" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="AA2" s="8" t="s">
+      <c r="AD2" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="AB2" s="8" t="s">
+      <c r="AE2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AK2" s="1">
+        <v>20</v>
+      </c>
+      <c r="AL2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AI2" s="1">
-        <v>20</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AO2" s="1">
+        <v>123</v>
+      </c>
+      <c r="AP2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="AM2" s="1">
+      <c r="AR2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AY2" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="BA2" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="BB2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="BC2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BD2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BE2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BF2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="BG2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BH2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="BI2" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="BK2" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="BL2" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="BM2" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="BN2" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="BO2" s="17">
+        <v>43972</v>
+      </c>
+      <c r="BP2">
         <v>123</v>
       </c>
-      <c r="AN2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AU2" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="AV2" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="AW2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AX2" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="AY2" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AZ2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="BA2" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="BB2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="BC2" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="BD2" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="BE2" s="1" t="s">
+      <c r="BQ2" t="s">
+        <v>205</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:71" s="10" customFormat="1">
+      <c r="C3" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="BF2" s="6"/>
-      <c r="BH2" s="9" t="s">
+      <c r="L3" s="12"/>
+      <c r="R3" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="U3" s="12"/>
+      <c r="AE3" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="BI2" s="9" t="s">
+      <c r="AF3" s="12"/>
+      <c r="AG3" s="12"/>
+      <c r="AH3" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="AU3" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="AV3" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="BA3" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="BB3" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="BE3" s="18" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="3" spans="1:61" s="10" customFormat="1">
-      <c r="C3" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="L3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="AC3" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="AD3" s="12"/>
-      <c r="AE3" s="12"/>
-      <c r="AF3" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="BB3" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="BC3" s="14"/>
-      <c r="BD3" s="14"/>
-      <c r="BE3" s="14"/>
+      <c r="BF3" s="18"/>
+      <c r="BG3" s="18"/>
+      <c r="BH3" s="18"/>
+      <c r="BN3" s="12"/>
+    </row>
+    <row r="6" spans="1:71">
+      <c r="E6" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="BB3:BE3"/>
+    <mergeCell ref="BE3:BH3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{FEB83603-4041-4AC3-87F2-87C79DF9B630}"/>
@@ -1377,44 +1592,49 @@
     <hyperlink ref="G2" r:id="rId7" display="Samuel@!" xr:uid="{4508698D-5125-4924-8669-2C63F2C79446}"/>
     <hyperlink ref="C2" r:id="rId8" xr:uid="{3584B448-8C19-4D61-B5C6-CF6CAD807BA7}"/>
     <hyperlink ref="Q2" r:id="rId9" xr:uid="{C3B18B62-FD76-49B4-AC64-952E552192A6}"/>
-    <hyperlink ref="T2" r:id="rId10" xr:uid="{A6D9E0E8-9647-4912-8849-2C709036FBFB}"/>
-    <hyperlink ref="U2" r:id="rId11" xr:uid="{03A9420C-BE4E-4CD7-83CA-712C4ADE84D8}"/>
-    <hyperlink ref="V2" r:id="rId12" xr:uid="{08ECC748-5948-4040-98CB-5F512E4B7301}"/>
-    <hyperlink ref="R2" r:id="rId13" xr:uid="{D0D49FFD-52B7-4610-8A3A-F6CE6EA95810}"/>
-    <hyperlink ref="Y2" r:id="rId14" xr:uid="{939F42D2-797F-4EF4-867E-7BFD07D6EFFC}"/>
-    <hyperlink ref="Z2" r:id="rId15" xr:uid="{EC4C6ACC-4058-435C-89FA-2275C3EB9357}"/>
-    <hyperlink ref="AA2" r:id="rId16" display="test@1234" xr:uid="{38B60C3F-7FD1-4B9C-873E-64BA8E8695E8}"/>
-    <hyperlink ref="AB2" r:id="rId17" xr:uid="{C052FBD8-54B3-4ABD-B212-87F718D2D335}"/>
-    <hyperlink ref="S2" r:id="rId18" xr:uid="{67F348E4-94FB-4ED2-B6E6-2FE03FD2EAE8}"/>
-    <hyperlink ref="AC2" r:id="rId19" xr:uid="{8B71A440-5A66-4098-B967-9D5375ED8181}"/>
-    <hyperlink ref="AE2" r:id="rId20" xr:uid="{A81C7D2B-2E01-42C3-8030-0EA608AD6665}"/>
-    <hyperlink ref="AD2" r:id="rId21" xr:uid="{AA5FFD45-DDB6-4311-869B-AD51F90222D0}"/>
-    <hyperlink ref="AG2" r:id="rId22" xr:uid="{EDC3C242-9D6E-4B14-BB15-E981BBFC1C28}"/>
-    <hyperlink ref="AH2" r:id="rId23" xr:uid="{9F03904E-A390-47AE-AFDD-655528A2B98A}"/>
-    <hyperlink ref="AO2" r:id="rId24" display="mailto:maf125@yopmail.com" xr:uid="{391B3587-9E43-46E8-9D66-76FAF1B11681}"/>
-    <hyperlink ref="AP2" r:id="rId25" xr:uid="{FC342C04-EEBA-42D2-A95E-B0C8FBCDD1E0}"/>
-    <hyperlink ref="AQ2" r:id="rId26" xr:uid="{94F1E8E9-1A05-4EE8-BE9F-133A92606266}"/>
-    <hyperlink ref="AS2" r:id="rId27" xr:uid="{371CF388-9097-484F-93F8-F79C9EFDBE19}"/>
-    <hyperlink ref="AT2" r:id="rId28" xr:uid="{04516551-9E75-4685-A3E0-2E32D9C110F7}"/>
-    <hyperlink ref="AU2" r:id="rId29" xr:uid="{5AB984D0-C0B8-49B6-99A2-C8C5E1A17DD9}"/>
-    <hyperlink ref="AV2" r:id="rId30" xr:uid="{9DEF9641-CF17-48D2-B650-590640FF1E02}"/>
-    <hyperlink ref="AF2" r:id="rId31" xr:uid="{C63DDE71-D130-4D74-B112-4B05CED4026E}"/>
-    <hyperlink ref="AW2" r:id="rId32" display="rasm.g@gmail.com" xr:uid="{6F6D1DA8-4F8C-4EE0-A9B0-2830798E1FE5}"/>
-    <hyperlink ref="AX2" r:id="rId33" xr:uid="{4EE4C7CC-2BE8-4AEF-B52A-67506C3A6C45}"/>
-    <hyperlink ref="AY2" r:id="rId34" xr:uid="{910E13F4-A439-45AB-82DB-3D21EA8FCF83}"/>
-    <hyperlink ref="BH2" r:id="rId35" xr:uid="{B66F5476-7F6E-461E-B40B-3630DFB2EFB0}"/>
-    <hyperlink ref="BI2" r:id="rId36" xr:uid="{DA2E6125-1460-4680-880E-0DAB589D8716}"/>
+    <hyperlink ref="V2" r:id="rId10" xr:uid="{A6D9E0E8-9647-4912-8849-2C709036FBFB}"/>
+    <hyperlink ref="W2" r:id="rId11" xr:uid="{03A9420C-BE4E-4CD7-83CA-712C4ADE84D8}"/>
+    <hyperlink ref="X2" r:id="rId12" xr:uid="{08ECC748-5948-4040-98CB-5F512E4B7301}"/>
+    <hyperlink ref="T2" r:id="rId13" xr:uid="{D0D49FFD-52B7-4610-8A3A-F6CE6EA95810}"/>
+    <hyperlink ref="AA2" r:id="rId14" xr:uid="{939F42D2-797F-4EF4-867E-7BFD07D6EFFC}"/>
+    <hyperlink ref="AB2" r:id="rId15" xr:uid="{EC4C6ACC-4058-435C-89FA-2275C3EB9357}"/>
+    <hyperlink ref="AC2" r:id="rId16" display="test@1234" xr:uid="{38B60C3F-7FD1-4B9C-873E-64BA8E8695E8}"/>
+    <hyperlink ref="AD2" r:id="rId17" xr:uid="{C052FBD8-54B3-4ABD-B212-87F718D2D335}"/>
+    <hyperlink ref="U2" r:id="rId18" xr:uid="{67F348E4-94FB-4ED2-B6E6-2FE03FD2EAE8}"/>
+    <hyperlink ref="AE2" r:id="rId19" xr:uid="{8B71A440-5A66-4098-B967-9D5375ED8181}"/>
+    <hyperlink ref="AG2" r:id="rId20" xr:uid="{A81C7D2B-2E01-42C3-8030-0EA608AD6665}"/>
+    <hyperlink ref="AF2" r:id="rId21" xr:uid="{AA5FFD45-DDB6-4311-869B-AD51F90222D0}"/>
+    <hyperlink ref="AI2" r:id="rId22" xr:uid="{EDC3C242-9D6E-4B14-BB15-E981BBFC1C28}"/>
+    <hyperlink ref="AJ2" r:id="rId23" xr:uid="{9F03904E-A390-47AE-AFDD-655528A2B98A}"/>
+    <hyperlink ref="AQ2" r:id="rId24" display="mailto:maf125@yopmail.com" xr:uid="{391B3587-9E43-46E8-9D66-76FAF1B11681}"/>
+    <hyperlink ref="AR2" r:id="rId25" xr:uid="{FC342C04-EEBA-42D2-A95E-B0C8FBCDD1E0}"/>
+    <hyperlink ref="AS2" r:id="rId26" xr:uid="{94F1E8E9-1A05-4EE8-BE9F-133A92606266}"/>
+    <hyperlink ref="AU2" r:id="rId27" xr:uid="{371CF388-9097-484F-93F8-F79C9EFDBE19}"/>
+    <hyperlink ref="AV2" r:id="rId28" xr:uid="{04516551-9E75-4685-A3E0-2E32D9C110F7}"/>
+    <hyperlink ref="AW2" r:id="rId29" xr:uid="{5AB984D0-C0B8-49B6-99A2-C8C5E1A17DD9}"/>
+    <hyperlink ref="AY2" r:id="rId30" xr:uid="{9DEF9641-CF17-48D2-B650-590640FF1E02}"/>
+    <hyperlink ref="AH2" r:id="rId31" xr:uid="{C63DDE71-D130-4D74-B112-4B05CED4026E}"/>
+    <hyperlink ref="AZ2" r:id="rId32" display="rasm.g@gmail.com" xr:uid="{6F6D1DA8-4F8C-4EE0-A9B0-2830798E1FE5}"/>
+    <hyperlink ref="BA2" r:id="rId33" xr:uid="{4EE4C7CC-2BE8-4AEF-B52A-67506C3A6C45}"/>
+    <hyperlink ref="BB2" r:id="rId34" xr:uid="{910E13F4-A439-45AB-82DB-3D21EA8FCF83}"/>
+    <hyperlink ref="BK2" r:id="rId35" xr:uid="{B66F5476-7F6E-461E-B40B-3630DFB2EFB0}"/>
+    <hyperlink ref="BL2" r:id="rId36" xr:uid="{DA2E6125-1460-4680-880E-0DAB589D8716}"/>
+    <hyperlink ref="AX2" r:id="rId37" xr:uid="{EE914E6A-EE92-4FF0-B07D-2B8ADCB4BCB8}"/>
+    <hyperlink ref="R2" r:id="rId38" xr:uid="{EB1698BB-CE31-4A8C-8A78-12B573EB1674}"/>
+    <hyperlink ref="S2" r:id="rId39" xr:uid="{A41C9E1F-4548-41A1-B8A5-9D37094640E3}"/>
+    <hyperlink ref="BI2" r:id="rId40" xr:uid="{12F3864C-B2F5-4EEE-9B59-1DB589969825}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId41"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7615949-9F3C-4DD2-B182-38B039D1A0DA}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1427,18 +1647,18 @@
     <col min="10" max="10" width="20.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>59</v>
@@ -1453,24 +1673,24 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1">
+    <row r="2" spans="1:8" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>109</v>
+        <v>62</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>169</v>
+        <v>210</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1489,43 +1709,49 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:2">
+      <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1533,157 +1759,209 @@
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>177</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9FB9B33-2A12-4BF6-9ABF-C5BE359B3CFF}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="C3" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E5" t="s">
         <v>138</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="F5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H5" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F4" t="s">
-        <v>140</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
+      <c r="G6" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" t="s">
-        <v>143</v>
-      </c>
-      <c r="F5" t="s">
-        <v>143</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
-        <v>147</v>
+      <c r="H7" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1691,6 +1969,7 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{5555CF94-AD36-4D4C-A94F-58406B4840EB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1706,42 +1985,42 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1769,42 +2048,42 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" t="s">
         <v>157</v>
-      </c>
-      <c r="B1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F2" t="s">
         <v>163</v>
-      </c>
-      <c r="B2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="E2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F2" t="s">
-        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>